<commit_message>
Added a script for running the arduino using my laptop
</commit_message>
<xml_diff>
--- a/sources/EnvironmentalData.xlsx
+++ b/sources/EnvironmentalData.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="17">
   <si>
     <t xml:space="preserve">Data Collected from Tayabas</t>
   </si>
@@ -46,7 +46,31 @@
     <t xml:space="preserve">Sample Size</t>
   </si>
   <si>
+    <t xml:space="preserve">a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">b</t>
+  </si>
+  <si>
     <t xml:space="preserve">Data Collected from Tagkawayan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Soil Moisture Readings (%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trial 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trial 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trial 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Setup A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Setup B</t>
   </si>
 </sst>
 </file>
@@ -57,12 +81,11 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.00%"/>
   </numFmts>
-  <fonts count="6">
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
+  <fonts count="18">
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -81,28 +104,145 @@
     </font>
     <font>
       <b val="true"/>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
+      <sz val="24"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i val="true"/>
+      <sz val="10"/>
+      <color rgb="FF808080"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u val="single"/>
+      <sz val="10"/>
+      <color rgb="FF0000EE"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF006600"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF996600"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFCC0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="14"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCFFCC"/>
+        <bgColor rgb="FFCCFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCCCC"/>
+        <bgColor rgb="FFDDDDDD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCC0000"/>
+        <bgColor rgb="FF800000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF000000"/>
+        <bgColor rgb="FF003300"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF808080"/>
+        <bgColor rgb="FF969696"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDDDDDD"/>
+        <bgColor rgb="FFFFCCCC"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -110,8 +250,23 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin">
+        <color rgb="FF808080"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF808080"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF808080"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF808080"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="20">
+  <cellStyleXfs count="37">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -135,6 +290,57 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -145,27 +351,27 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -182,14 +388,91 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="23">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Heading" xfId="20" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Heading 1" xfId="21" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Heading 2" xfId="22" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Text" xfId="23" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Note" xfId="24" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Footnote" xfId="25" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Hyperlink" xfId="26" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Status" xfId="27" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Good" xfId="28" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Neutral" xfId="29" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Bad" xfId="30" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Warning" xfId="31" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Error" xfId="32" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent" xfId="33" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent 1" xfId="34" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent 2" xfId="35" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent 3" xfId="36" builtinId="53" customBuiltin="true"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFCC0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000EE"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF006600"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF996600"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFDDDDDD"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCCCC"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -198,10 +481,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J23"/>
+  <dimension ref="A1:O31"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B24" activeCellId="0" sqref="B24"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C30" activeCellId="0" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -368,14 +651,75 @@
         <v>860</v>
       </c>
     </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N11" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M12" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="N12" s="1" t="n">
+        <v>123</v>
+      </c>
+      <c r="O12" s="1" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M13" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="N13" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="O13" s="1" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M14" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="N14" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="O14" s="1" t="n">
+        <v>4</v>
+      </c>
+    </row>
     <row r="15" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C15" s="4" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
+      <c r="M15" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="N15" s="1" t="n">
+        <v>43</v>
+      </c>
+      <c r="O15" s="1" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M16" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="N16" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="O16" s="1" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="5" t="s">
@@ -392,6 +736,26 @@
       <c r="H17" s="7"/>
       <c r="I17" s="7"/>
       <c r="J17" s="7"/>
+      <c r="M17" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="N17" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="O17" s="1" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M18" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="N18" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="O18" s="1" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="s">
@@ -500,14 +864,51 @@
         <v>84.4204873119874</v>
       </c>
     </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B28" s="6"/>
+      <c r="C28" s="6"/>
+      <c r="D28" s="6"/>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0"/>
+      <c r="B29" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B30" s="1" t="n">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B31" s="1" t="n">
+        <v>62</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
     <mergeCell ref="C2:G2"/>
     <mergeCell ref="A4:D4"/>
     <mergeCell ref="F4:J4"/>
     <mergeCell ref="C15:G15"/>
     <mergeCell ref="A17:D17"/>
     <mergeCell ref="F17:J17"/>
+    <mergeCell ref="A28:D28"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>